<commit_message>
WIP Hooking excel paring into selenium completion, now selects by most recent modifed file aka the one selenium downloaded :)
</commit_message>
<xml_diff>
--- a/src/Excel Files/productSearch9_3Page1.xlsx
+++ b/src/Excel Files/productSearch9_3Page1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\sourceclub\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\sourceclub\src\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2449,7 +2449,7 @@
         <v>23.87</v>
       </c>
       <c r="G28">
-        <v>11.42</v>
+        <v>11.32</v>
       </c>
       <c r="H28">
         <v>12.45</v>

</xml_diff>